<commit_message>
Friday update to my crap
</commit_message>
<xml_diff>
--- a/SCP_Master_Data_Source.xlsx
+++ b/SCP_Master_Data_Source.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rob\Documents\Telework\telework_projects\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F1A1292-C076-48B9-81AF-4E58822BC44A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D127FD3-905D-48D2-B6A9-B9D6C3E7A470}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12252" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="202">
   <si>
     <t>acor</t>
   </si>
@@ -411,39 +411,9 @@
     <t>vendor</t>
   </si>
   <si>
-    <t>empty</t>
-  </si>
-  <si>
-    <t>OP16-004</t>
-  </si>
-  <si>
-    <t>MP17-053</t>
-  </si>
-  <si>
-    <t>MP14-022</t>
-  </si>
-  <si>
-    <t>MP14-058</t>
-  </si>
-  <si>
-    <t>D216-027</t>
-  </si>
-  <si>
     <t>2016-08-31T05:00:00.000Z</t>
   </si>
   <si>
-    <t>comments</t>
-  </si>
-  <si>
-    <t>IGCE: $ 1139164.45 "ammendment only updated, etc…"</t>
-  </si>
-  <si>
-    <t>"committed to GSA"</t>
-  </si>
-  <si>
-    <t>NOT SET</t>
-  </si>
-  <si>
     <t>interagency</t>
   </si>
   <si>
@@ -471,45 +441,9 @@
     <t>2019-12-31T05:00:00.000Z</t>
   </si>
   <si>
-    <t>HM157515C0018</t>
-  </si>
-  <si>
-    <t>HM157515C0019</t>
-  </si>
-  <si>
-    <t>HM157515C0020</t>
-  </si>
-  <si>
-    <t>HM157515C0021</t>
-  </si>
-  <si>
-    <t>HM157515C0022</t>
-  </si>
-  <si>
-    <t>Smith, Jack</t>
-  </si>
-  <si>
-    <t>McGrus, Sarah</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Jaeger, Bob</t>
-  </si>
-  <si>
-    <t>Forrest, Green</t>
-  </si>
-  <si>
-    <t>Non-GGI-GDS</t>
-  </si>
-  <si>
     <t>MIPR</t>
   </si>
   <si>
-    <t>Janus-Geo</t>
-  </si>
-  <si>
     <t>Stand Alone</t>
   </si>
   <si>
@@ -525,27 +459,6 @@
     <t>options</t>
   </si>
   <si>
-    <t>APAS - Flight Procedures</t>
-  </si>
-  <si>
-    <t>CLIN 4329</t>
-  </si>
-  <si>
-    <t>SFH</t>
-  </si>
-  <si>
-    <t>SFN</t>
-  </si>
-  <si>
-    <t>SC</t>
-  </si>
-  <si>
-    <t>SFG</t>
-  </si>
-  <si>
-    <t>SFA</t>
-  </si>
-  <si>
     <t>Awarded/Obligated</t>
   </si>
   <si>
@@ -576,35 +489,158 @@
     <t>2020-01-28T05:00:00.000Z</t>
   </si>
   <si>
-    <t>HM157518F0235</t>
-  </si>
-  <si>
-    <t>Kirkland</t>
-  </si>
-  <si>
     <t>date</t>
   </si>
   <si>
-    <t>USGS</t>
-  </si>
-  <si>
-    <t>DTIC</t>
-  </si>
-  <si>
-    <t>Harris</t>
-  </si>
-  <si>
-    <t>BAE</t>
-  </si>
-  <si>
-    <t>Hexagon</t>
+    <t>XXXX-001</t>
+  </si>
+  <si>
+    <t>XXXX-002</t>
+  </si>
+  <si>
+    <t>XXXX-003</t>
+  </si>
+  <si>
+    <t>XXXX-004</t>
+  </si>
+  <si>
+    <t>XXXX-005</t>
+  </si>
+  <si>
+    <t>Rando comment 1</t>
+  </si>
+  <si>
+    <t>Rando comment 2</t>
+  </si>
+  <si>
+    <t>Rando comment 3</t>
+  </si>
+  <si>
+    <t>Rando comment 4</t>
+  </si>
+  <si>
+    <t>Rando comment 5</t>
+  </si>
+  <si>
+    <t>XX123456X1234</t>
+  </si>
+  <si>
+    <t>XX123456X1235</t>
+  </si>
+  <si>
+    <t>XX123456X1236</t>
+  </si>
+  <si>
+    <t>XX123456X1237</t>
+  </si>
+  <si>
+    <t>XX123456X1238</t>
+  </si>
+  <si>
+    <t>Joseph, Curtis</t>
+  </si>
+  <si>
+    <t>Fuhr, Grant</t>
+  </si>
+  <si>
+    <t>Riendeau, Vince</t>
+  </si>
+  <si>
+    <t>Hebert, Guy</t>
+  </si>
+  <si>
+    <t>Binnington, Jordan</t>
+  </si>
+  <si>
+    <t>Fake-Geo</t>
+  </si>
+  <si>
+    <t>Safety</t>
+  </si>
+  <si>
+    <t>CLIN 0001</t>
+  </si>
+  <si>
+    <t>ABC</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>BBC</t>
+  </si>
+  <si>
+    <t>CNN</t>
+  </si>
+  <si>
+    <t>ESPN</t>
+  </si>
+  <si>
+    <t>XX11-001</t>
+  </si>
+  <si>
+    <t>XX11-002</t>
+  </si>
+  <si>
+    <t>XX11-003</t>
+  </si>
+  <si>
+    <t>XX11-004</t>
+  </si>
+  <si>
+    <t>XX11-005</t>
+  </si>
+  <si>
+    <t>AB123456X0000</t>
+  </si>
+  <si>
+    <t>AB123456X0001</t>
+  </si>
+  <si>
+    <t>AB123456X0002</t>
+  </si>
+  <si>
+    <t>AB123456X0003</t>
+  </si>
+  <si>
+    <t>AB123456X0004</t>
+  </si>
+  <si>
+    <t>Fake</t>
+  </si>
+  <si>
+    <t>Names</t>
+  </si>
+  <si>
+    <t>Here</t>
+  </si>
+  <si>
+    <t>And</t>
+  </si>
+  <si>
+    <t>Amazon</t>
+  </si>
+  <si>
+    <t>Microsoft</t>
+  </si>
+  <si>
+    <t>Sun</t>
+  </si>
+  <si>
+    <t>Apple</t>
+  </si>
+  <si>
+    <t>It</t>
+  </si>
+  <si>
+    <t>Doesn’tMatter</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -735,6 +771,12 @@
     <font>
       <sz val="11"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1412,8 +1454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DX7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="DB1" workbookViewId="0">
-      <selection activeCell="X1" sqref="X1:X1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="DX8" sqref="DX8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1427,13 +1469,13 @@
     <col min="8" max="8" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="8.109375" customWidth="1"/>
-    <col min="12" max="12" width="10.44140625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.21875" customWidth="1"/>
     <col min="13" max="13" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="21.6640625" customWidth="1"/>
     <col min="15" max="15" width="14.5546875" customWidth="1"/>
     <col min="16" max="16" width="13.6640625" customWidth="1"/>
     <col min="17" max="17" width="18" customWidth="1"/>
-    <col min="18" max="18" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16.109375" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="16.88671875" customWidth="1"/>
     <col min="20" max="20" width="13.33203125" customWidth="1"/>
     <col min="21" max="21" width="14.44140625" customWidth="1"/>
@@ -1442,8 +1484,14 @@
     <col min="25" max="25" width="23.21875" bestFit="1" customWidth="1"/>
     <col min="26" max="26" width="21" customWidth="1"/>
     <col min="27" max="27" width="20.5546875" customWidth="1"/>
+    <col min="29" max="29" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="23.77734375" customWidth="1"/>
     <col min="59" max="59" width="10" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="23.21875" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14.88671875" bestFit="1" customWidth="1"/>
     <col min="119" max="119" width="10" bestFit="1" customWidth="1"/>
+    <col min="128" max="128" width="12.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:128" s="2" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
@@ -1836,107 +1884,47 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>127</v>
-      </c>
       <c r="C2" t="s">
-        <v>128</v>
-      </c>
-      <c r="D2" t="s">
-        <v>127</v>
-      </c>
-      <c r="E2" t="s">
-        <v>127</v>
+        <v>154</v>
       </c>
       <c r="F2" t="b">
         <v>1</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>127</v>
       </c>
-      <c r="H2" t="s">
-        <v>133</v>
-      </c>
       <c r="I2" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="J2" t="s">
-        <v>127</v>
-      </c>
-      <c r="K2" t="s">
-        <v>127</v>
+        <v>159</v>
       </c>
       <c r="L2" t="s">
+        <v>128</v>
+      </c>
+      <c r="M2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>164</v>
+      </c>
+      <c r="R2" t="s">
+        <v>169</v>
+      </c>
+      <c r="U2" t="s">
         <v>137</v>
       </c>
-      <c r="M2" t="s">
+      <c r="Y2" t="s">
         <v>139</v>
       </c>
-      <c r="N2" t="s">
-        <v>127</v>
-      </c>
-      <c r="O2" t="s">
-        <v>127</v>
-      </c>
-      <c r="P2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>147</v>
-      </c>
-      <c r="R2" t="s">
-        <v>152</v>
-      </c>
-      <c r="S2" t="s">
-        <v>127</v>
-      </c>
-      <c r="T2" t="s">
-        <v>127</v>
-      </c>
-      <c r="U2" t="s">
-        <v>157</v>
-      </c>
-      <c r="V2" t="s">
-        <v>127</v>
-      </c>
-      <c r="W2" t="s">
-        <v>127</v>
-      </c>
-      <c r="X2" t="s">
-        <v>127</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>161</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>127</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>127</v>
-      </c>
       <c r="AC2" s="1" t="s">
-        <v>162</v>
+        <v>140</v>
       </c>
       <c r="AI2" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
       <c r="AM2">
         <v>2016</v>
       </c>
-      <c r="AQ2">
-        <v>0</v>
-      </c>
-      <c r="AR2">
-        <v>0</v>
-      </c>
-      <c r="AS2">
-        <v>0</v>
-      </c>
       <c r="BF2" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
       <c r="BG2">
         <v>0</v>
@@ -1945,22 +1933,25 @@
         <v>1</v>
       </c>
       <c r="BM2" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="BP2" t="s">
-        <v>176</v>
+        <v>147</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>187</v>
       </c>
       <c r="CD2">
         <v>0</v>
       </c>
       <c r="CH2" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="CK2" t="s">
-        <v>154</v>
+        <v>192</v>
       </c>
       <c r="CM2" t="s">
-        <v>184</v>
+        <v>153</v>
       </c>
       <c r="CT2" t="b">
         <v>0</v>
@@ -1969,63 +1960,54 @@
         <v>0</v>
       </c>
       <c r="DX2" t="s">
-        <v>189</v>
+        <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:128" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:128" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>129</v>
+        <v>155</v>
       </c>
       <c r="F3" t="b">
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>140</v>
+        <v>130</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>135</v>
+        <v>160</v>
       </c>
       <c r="L3" t="s">
+        <v>128</v>
+      </c>
+      <c r="M3" t="s">
+        <v>129</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>165</v>
+      </c>
+      <c r="R3" t="s">
+        <v>170</v>
+      </c>
+      <c r="U3" t="s">
         <v>138</v>
       </c>
-      <c r="M3" t="s">
+      <c r="Y3" t="s">
         <v>139</v>
       </c>
-      <c r="Q3" t="s">
-        <v>148</v>
-      </c>
-      <c r="R3" t="s">
-        <v>153</v>
-      </c>
-      <c r="U3" t="s">
-        <v>158</v>
-      </c>
-      <c r="Y3" t="s">
-        <v>161</v>
-      </c>
       <c r="AC3" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="AI3" t="s">
-        <v>167</v>
+        <v>178</v>
       </c>
       <c r="AM3">
         <v>2017</v>
       </c>
-      <c r="AQ3">
-        <v>0</v>
-      </c>
-      <c r="AR3">
-        <v>0</v>
-      </c>
-      <c r="AS3">
-        <v>0</v>
-      </c>
       <c r="BF3" t="s">
-        <v>129</v>
+        <v>183</v>
       </c>
       <c r="BG3">
         <v>2060000</v>
@@ -2034,25 +2016,28 @@
         <v>1</v>
       </c>
       <c r="BM3" t="s">
-        <v>173</v>
+        <v>144</v>
       </c>
       <c r="BP3" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="BQ3" t="s">
-        <v>178</v>
+        <v>149</v>
       </c>
       <c r="CA3" t="s">
-        <v>182</v>
+        <v>188</v>
       </c>
       <c r="CD3">
         <v>83.7</v>
       </c>
       <c r="CK3" t="s">
-        <v>183</v>
+        <v>193</v>
       </c>
       <c r="DO3">
         <v>181000000</v>
+      </c>
+      <c r="DX3" t="s">
+        <v>197</v>
       </c>
     </row>
     <row r="4" spans="1:128" x14ac:dyDescent="0.3">
@@ -2060,52 +2045,46 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="F4" t="b">
         <v>1</v>
       </c>
       <c r="H4" t="s">
-        <v>141</v>
+        <v>131</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>161</v>
       </c>
       <c r="L4" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M4" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="Q4" t="s">
-        <v>149</v>
+        <v>166</v>
       </c>
       <c r="R4" t="s">
-        <v>154</v>
+        <v>171</v>
       </c>
       <c r="U4" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="Y4" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="AC4" t="s">
-        <v>164</v>
+        <v>142</v>
       </c>
       <c r="AI4" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
       <c r="AM4">
         <v>2014</v>
       </c>
-      <c r="AQ4">
-        <v>0</v>
-      </c>
-      <c r="AR4">
-        <v>0</v>
-      </c>
-      <c r="AS4">
-        <v>0</v>
-      </c>
       <c r="BF4" t="s">
-        <v>130</v>
+        <v>184</v>
       </c>
       <c r="BG4">
         <v>338232043</v>
@@ -2114,22 +2093,28 @@
         <v>1</v>
       </c>
       <c r="BM4" t="s">
-        <v>175</v>
+        <v>146</v>
       </c>
       <c r="BP4" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="BQ4" t="s">
-        <v>179</v>
+        <v>150</v>
+      </c>
+      <c r="CA4" t="s">
+        <v>189</v>
       </c>
       <c r="CD4">
         <v>100</v>
       </c>
+      <c r="CK4" t="s">
+        <v>194</v>
+      </c>
       <c r="DO4">
         <v>0</v>
       </c>
       <c r="DX4" t="s">
-        <v>185</v>
+        <v>198</v>
       </c>
     </row>
     <row r="5" spans="1:128" x14ac:dyDescent="0.3">
@@ -2137,52 +2122,46 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>131</v>
+        <v>157</v>
       </c>
       <c r="F5" t="b">
         <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>142</v>
+        <v>132</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>162</v>
       </c>
       <c r="L5" t="s">
-        <v>138</v>
+        <v>128</v>
       </c>
       <c r="M5" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="Q5" t="s">
-        <v>150</v>
+        <v>167</v>
       </c>
       <c r="R5" t="s">
-        <v>155</v>
+        <v>172</v>
       </c>
       <c r="U5" t="s">
-        <v>159</v>
+        <v>174</v>
       </c>
       <c r="Y5" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="AC5" t="s">
-        <v>165</v>
+        <v>175</v>
       </c>
       <c r="AI5" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
       <c r="AM5">
         <v>2019</v>
       </c>
-      <c r="AQ5">
-        <v>0</v>
-      </c>
-      <c r="AR5">
-        <v>0</v>
-      </c>
-      <c r="AS5">
-        <v>0</v>
-      </c>
       <c r="BF5" t="s">
-        <v>131</v>
+        <v>185</v>
       </c>
       <c r="BG5">
         <v>8334673</v>
@@ -2191,19 +2170,25 @@
         <v>1</v>
       </c>
       <c r="BM5" t="s">
-        <v>174</v>
+        <v>145</v>
       </c>
       <c r="BP5" t="s">
-        <v>177</v>
+        <v>148</v>
       </c>
       <c r="BQ5" t="s">
-        <v>180</v>
+        <v>151</v>
+      </c>
+      <c r="CA5" t="s">
+        <v>190</v>
+      </c>
+      <c r="CK5" t="s">
+        <v>195</v>
       </c>
       <c r="DO5">
         <v>7214900</v>
       </c>
       <c r="DX5" t="s">
-        <v>186</v>
+        <v>199</v>
       </c>
     </row>
     <row r="6" spans="1:128" x14ac:dyDescent="0.3">
@@ -2211,55 +2196,46 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>132</v>
+        <v>158</v>
       </c>
       <c r="F6" t="b">
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>143</v>
+        <v>133</v>
       </c>
       <c r="I6" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="L6" t="s">
+        <v>128</v>
+      </c>
+      <c r="M6" t="s">
         <v>136</v>
       </c>
-      <c r="L6" t="s">
-        <v>137</v>
-      </c>
-      <c r="M6" t="s">
-        <v>146</v>
-      </c>
       <c r="Q6" t="s">
-        <v>151</v>
+        <v>168</v>
       </c>
       <c r="R6" t="s">
-        <v>156</v>
+        <v>173</v>
       </c>
       <c r="U6" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="Y6" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="AC6" t="s">
-        <v>166</v>
+        <v>176</v>
       </c>
       <c r="AI6" t="s">
-        <v>171</v>
+        <v>181</v>
       </c>
       <c r="AM6">
         <v>2020</v>
       </c>
-      <c r="AQ6">
-        <v>0</v>
-      </c>
-      <c r="AR6">
-        <v>0</v>
-      </c>
-      <c r="AS6">
-        <v>0</v>
-      </c>
       <c r="BF6" t="s">
-        <v>132</v>
+        <v>186</v>
       </c>
       <c r="BG6">
         <v>15478420</v>
@@ -2268,33 +2244,37 @@
         <v>1</v>
       </c>
       <c r="BM6" t="s">
-        <v>172</v>
+        <v>143</v>
       </c>
       <c r="BP6" t="s">
-        <v>176</v>
+        <v>147</v>
       </c>
       <c r="BQ6" t="s">
-        <v>181</v>
+        <v>152</v>
+      </c>
+      <c r="CA6" t="s">
+        <v>191</v>
+      </c>
+      <c r="CK6" t="s">
+        <v>194</v>
       </c>
       <c r="DO6">
         <v>15784782</v>
       </c>
       <c r="DX6" t="s">
-        <v>187</v>
+        <v>200</v>
       </c>
     </row>
     <row r="7" spans="1:128" x14ac:dyDescent="0.3">
-      <c r="AQ7">
-        <v>0</v>
-      </c>
       <c r="BL7" t="b">
         <v>1</v>
       </c>
       <c r="DX7" t="s">
-        <v>188</v>
+        <v>201</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="18" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.5" header="0.3" footer="0.3"/>
   <pageSetup scale="70" orientation="landscape" r:id="rId1"/>
   <headerFooter>

</xml_diff>